<commit_message>
chapter 5 initial draft
</commit_message>
<xml_diff>
--- a/figures/5_Ascent/BarChart.xlsx
+++ b/figures/5_Ascent/BarChart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Dynamic Pressure</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>m2</t>
+  </si>
+  <si>
+    <t>Cd3</t>
   </si>
 </sst>
 </file>
@@ -181,28 +184,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$G$1</c:f>
+              <c:f>Sheet1!$A$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>Cd3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Dynamic Pressure</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>mFuel2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>m2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Cd</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Isp</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>T3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>m3</c:v>
                 </c:pt>
               </c:strCache>
@@ -210,29 +216,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$G$2</c:f>
+              <c:f>Sheet1!$A$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2.6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -249,11 +258,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="439498128"/>
-        <c:axId val="439498520"/>
+        <c:axId val="505213816"/>
+        <c:axId val="505214200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="439498128"/>
+        <c:axId val="505213816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -296,7 +305,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439498520"/>
+        <c:crossAx val="505214200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -304,7 +313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="439498520"/>
+        <c:axId val="505214200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +364,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439498128"/>
+        <c:crossAx val="505213816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1269,57 +1278,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0.02</v>
+      </c>
+      <c r="B2">
         <v>0.36</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.7</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1.5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.9</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.6</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>3.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did a lot of comments
</commit_message>
<xml_diff>
--- a/figures/5_Ascent/BarChart.xlsx
+++ b/figures/5_Ascent/BarChart.xlsx
@@ -44,13 +44,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,20 +127,15 @@
                     <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Payload Variation</a:t>
+              <a:t>Payload Variation (kg) per % Parameter Variation</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> (kg) per % Parameter Variation</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -158,9 +160,9 @@
                   <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -203,32 +205,6 @@
                   <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:sysClr val="windowText" lastClr="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -271,9 +247,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -281,9 +255,9 @@
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -393,11 +367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="219788224"/>
-        <c:axId val="220158968"/>
+        <c:axId val="453712056"/>
+        <c:axId val="453712840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219788224"/>
+        <c:axId val="453712056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,15 +406,15 @@
                     <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220158968"/>
+        <c:crossAx val="453712840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -448,7 +422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220158968"/>
+        <c:axId val="453712840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-2"/>
@@ -504,15 +478,15 @@
                     <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219788224"/>
+        <c:crossAx val="453712056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -548,7 +522,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1495,66 +1472,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0.02</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0.7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.9</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>-1.5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>-1.9</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>4.5999999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>